<commit_message>
FMR Excel Test File Update
</commit_message>
<xml_diff>
--- a/Crawlers/FMR_Crawler_Test_Excel.xlsx
+++ b/Crawlers/FMR_Crawler_Test_Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python\221Project\SectionM8-Demo-Fall2025\Crawlers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D82A86E-F4CA-42BF-9321-3E5831B7663B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F40ECFD3-BD1B-47C0-AD40-AE67EAC22C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:W8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="W8" sqref="A1:W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>